<commit_message>
added rudimentary gui for uploading new results/fasta
</commit_message>
<xml_diff>
--- a/utility/testing/edited_20240129-PepsinDigestionformatted.xlsx
+++ b/utility/testing/edited_20240129-PepsinDigestionformatted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhatk\PycharmProjects\sarlacc\utility\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880FE68D-EE33-4B05-93BB-FD866582DF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A58B1AE-B4C5-4878-9E17-B872A459C4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="6">
   <si>
     <t>Sequence</t>
   </si>
@@ -31,7 +31,13 @@
     <t>End</t>
   </si>
   <si>
-    <t>MSEW</t>
+    <t>WKAMV</t>
+  </si>
+  <si>
+    <t>WWKAMV</t>
+  </si>
+  <si>
+    <t>MSEWW</t>
   </si>
 </sst>
 </file>
@@ -872,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C22"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -896,10 +902,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -907,10 +913,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -918,10 +924,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -929,10 +935,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -940,10 +946,10 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -951,10 +957,10 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -962,10 +968,10 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -973,10 +979,10 @@
         <v>3</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -984,10 +990,10 @@
         <v>3</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
@@ -995,10 +1001,10 @@
         <v>3</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
@@ -1006,10 +1012,10 @@
         <v>3</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -1017,10 +1023,10 @@
         <v>3</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -1028,10 +1034,10 @@
         <v>3</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
@@ -1039,10 +1045,10 @@
         <v>3</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
@@ -1050,10 +1056,10 @@
         <v>3</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
@@ -1061,10 +1067,10 @@
         <v>3</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
@@ -1072,10 +1078,10 @@
         <v>3</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
@@ -1083,10 +1089,10 @@
         <v>3</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
@@ -1094,10 +1100,10 @@
         <v>3</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
@@ -1105,10 +1111,10 @@
         <v>3</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
@@ -1116,10 +1122,76 @@
         <v>3</v>
       </c>
       <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28">
         <v>1</v>
       </c>
-      <c r="C22">
-        <v>4</v>
+      <c r="C28">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>